<commit_message>
will finish when i am on campus and have SPSS & SAS
</commit_message>
<xml_diff>
--- a/mote_progress.xlsx
+++ b/mote_progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Harrisburg University/Research/2 projects/MOTE-papers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber Gillenwaters\Documents\GitHub\MOTE-papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{BE6E76A7-2715-40AE-B406-F9D210E693DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{2DCF91A9-5346-8140-98AE-C863AEBB8802}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0430708E-762F-4163-9748-2A4050C19F93}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23260" yWindow="460" windowWidth="25600" windowHeight="14400" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D46B8A7-845A-3943-97E8-0D703E8368C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="111">
   <si>
     <t>apa.R</t>
   </si>
@@ -347,6 +347,21 @@
   </si>
   <si>
     <t>fix the SAS output, it's wrong - can we figure out why the JASP output says 1 and 157, while the SPSS output says 1, 156 (this is right)</t>
+  </si>
+  <si>
+    <t>NEEDS NEW SAS PIC</t>
+  </si>
+  <si>
+    <t>NEED TO CHECK SPSS</t>
+  </si>
+  <si>
+    <t>NEEDS SPSS &amp; SAS PIC</t>
+  </si>
+  <si>
+    <t>amber comments</t>
+  </si>
+  <si>
+    <t>This vid shows a 2 way on the dataset. (https://www.youtube.com/watch?v=GgO1APyHtak) but the vid on the Shiny app was a threeway (https://www.youtube.com/watch?time_continue=334&amp;v=Y1piNdNdMbc) I think I'm gonna change the SPSS output instead to  match the Shiny app vid. Changed example text NEEDS SAS PIC</t>
   </si>
 </sst>
 </file>
@@ -432,14 +447,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -760,38 +775,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD9EC07C-AD64-B046-8A0B-7C71E03C2500}">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="19" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="36.5" customWidth="1"/>
-    <col min="10" max="10" width="54.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="36.44140625" customWidth="1"/>
+    <col min="11" max="11" width="54.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="6"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" ht="34">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" ht="30">
       <c r="A2" s="7" t="s">
         <v>77</v>
       </c>
@@ -820,10 +836,13 @@
         <v>99</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17">
+    <row r="3" spans="1:11">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -851,11 +870,12 @@
       <c r="I3" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17">
+      <c r="J3" s="5"/>
+      <c r="K3" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -883,11 +903,12 @@
       <c r="I4" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17">
+      <c r="J4" s="5"/>
+      <c r="K4" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -915,11 +936,12 @@
       <c r="I5" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="34">
+      <c r="J5" s="5"/>
+      <c r="K5" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -944,14 +966,17 @@
       <c r="H6" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="17">
+      <c r="J6" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -979,11 +1004,12 @@
       <c r="I7" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="17">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -1011,11 +1037,12 @@
       <c r="I8" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="17">
+      <c r="J8" s="5"/>
+      <c r="K8" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1043,11 +1070,12 @@
       <c r="I9" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17">
+      <c r="J9" s="5"/>
+      <c r="K9" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1075,11 +1103,12 @@
       <c r="I10" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17">
+      <c r="J10" s="5"/>
+      <c r="K10" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
@@ -1107,11 +1136,12 @@
       <c r="I11" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="17">
+      <c r="J11" s="5"/>
+      <c r="K11" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
@@ -1139,11 +1169,12 @@
       <c r="I12" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17">
+      <c r="J12" s="5"/>
+      <c r="K12" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
@@ -1171,11 +1202,12 @@
       <c r="I13" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="17">
+      <c r="J13" s="5"/>
+      <c r="K13" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
@@ -1203,11 +1235,12 @@
       <c r="I14" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="17">
+      <c r="J14" s="5"/>
+      <c r="K14" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="8" t="s">
         <v>11</v>
       </c>
@@ -1235,11 +1268,12 @@
       <c r="I15" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J15" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17">
+      <c r="J15" s="5"/>
+      <c r="K15" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="8" t="s">
         <v>12</v>
       </c>
@@ -1267,11 +1301,12 @@
       <c r="I16" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="17">
+      <c r="J16" s="5"/>
+      <c r="K16" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
@@ -1299,11 +1334,12 @@
       <c r="I17" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17">
+      <c r="J17" s="5"/>
+      <c r="K17" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
@@ -1331,11 +1367,12 @@
       <c r="I18" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="17">
+      <c r="J18" s="5"/>
+      <c r="K18" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
@@ -1363,11 +1400,12 @@
       <c r="I19" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="17">
+      <c r="J19" s="5"/>
+      <c r="K19" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
@@ -1395,11 +1433,12 @@
       <c r="I20" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J20" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="142" customHeight="1">
+      <c r="J20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="141.94999999999999" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
@@ -1424,14 +1463,17 @@
       <c r="H21" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="I21" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="68">
+      <c r="J21" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1456,14 +1498,17 @@
       <c r="H22" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="I22" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="J22" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="17">
+      <c r="J22" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
@@ -1489,8 +1534,9 @@
         <v>58</v>
       </c>
       <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" ht="17">
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
@@ -1518,11 +1564,12 @@
       <c r="I24" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J24" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="17">
+      <c r="J24" s="5"/>
+      <c r="K24" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
@@ -1550,11 +1597,12 @@
       <c r="I25" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="68">
+      <c r="J25" s="5"/>
+      <c r="K25" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="60">
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
@@ -1579,14 +1627,17 @@
       <c r="H26" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="I26" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="J26" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="17">
+      <c r="J26" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
@@ -1614,11 +1665,12 @@
       <c r="I27" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J27" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="68">
+      <c r="J27" s="5"/>
+      <c r="K27" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="60">
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
@@ -1643,14 +1695,17 @@
       <c r="H28" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I28" s="11" t="s">
+      <c r="I28" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="J28" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="85">
+      <c r="J28" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="75">
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
@@ -1675,14 +1730,17 @@
       <c r="H29" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I29" s="11" t="s">
+      <c r="I29" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="J29" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="17">
+      <c r="J29" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="8" t="s">
         <v>28</v>
       </c>
@@ -1710,11 +1768,12 @@
       <c r="I30" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J30" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="J30" s="5"/>
+      <c r="K30" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="1"/>
     </row>
     <row r="33" spans="1:1">
@@ -1789,7 +1848,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1804,16 +1863,16 @@
       <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="7" width="27.1640625" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" customWidth="1"/>
+    <col min="6" max="7" width="27.109375" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2072,7 +2131,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="85">
+    <row r="12" spans="1:11" ht="75">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2118,7 +2177,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="119">
+    <row r="14" spans="1:11" ht="105">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2142,7 +2201,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="68">
+    <row r="15" spans="1:11" ht="60">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2166,7 +2225,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="51">
+    <row r="16" spans="1:11" ht="30">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2190,7 +2249,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>14</v>
       </c>

</xml_diff>